<commit_message>
Fix year % 1 schedule generation
</commit_message>
<xml_diff>
--- a/Celarix.JustForFun.FootballSimulator/Valid 40-Team NFL Division Matchups.xlsx
+++ b/Celarix.JustForFun.FootballSimulator/Valid 40-Team NFL Division Matchups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Misc\Celarix.JustForFun.FootballSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B836820-3E94-42BB-9188-B4EE7B481B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC17398-8A51-4186-A7C0-538C19221828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{15257DEB-FCC1-4014-92A7-EF091E06D8A0}"/>
+    <workbookView xWindow="-28920" yWindow="-2850" windowWidth="29040" windowHeight="15840" xr2:uid="{15257DEB-FCC1-4014-92A7-EF091E06D8A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="37">
   <si>
     <t>First year</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>West/East</t>
-  </si>
-  <si>
-    <t>East/South</t>
   </si>
   <si>
     <t>North/South</t>
@@ -222,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -230,7 +227,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E05959-7028-4626-B827-E37BA2F8E9B7}">
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,7 +1014,7 @@
         <v>20</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>21</v>
@@ -1048,7 +1044,7 @@
         <v>15</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T11" s="4" t="s">
         <v>16</v>
@@ -1128,13 +1124,13 @@
         <v>20</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>19</v>
@@ -1152,19 +1148,19 @@
         <v>17</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P13" s="3" t="s">
         <v>14</v>
@@ -1182,7 +1178,7 @@
         <v>15</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1390,13 +1386,13 @@
         <v>17</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>19</v>
@@ -1408,7 +1404,7 @@
         <v>20</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>13</v>
@@ -1420,13 +1416,13 @@
         <v>14</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R17" s="4" t="s">
         <v>16</v>
@@ -1438,7 +1434,7 @@
         <v>12</v>
       </c>
       <c r="U17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -1511,7 +1507,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>20</v>
@@ -1523,57 +1519,50 @@
         <v>21</v>
       </c>
       <c r="G19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K19" s="3" t="s">
+      <c r="N19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O19" s="3" t="s">
+      <c r="T19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="U19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="P19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q19" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="R19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="S19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="T19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="U19" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="M20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="U20" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>